<commit_message>
parkinsons telemonitering dataset removede
</commit_message>
<xml_diff>
--- a/Datasets.xlsx
+++ b/Datasets.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Btech\sem8 Aroygasathi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Btech\sem8 Aroygasathi\ArogyaSathi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2718EC4-D574-4AB5-B3F5-ACB7402FD745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F94861-B51C-44DA-9359-050F9BAD958D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Dataset study</t>
   </si>
@@ -194,9 +194,6 @@
     <t>risk of coronary heart disease</t>
   </si>
   <si>
-    <t>16 columns</t>
-  </si>
-  <si>
     <t>Pima Indians Diabetes Database</t>
   </si>
   <si>
@@ -206,26 +203,33 @@
     <t>diabetes</t>
   </si>
   <si>
-    <t>9 columns</t>
-  </si>
-  <si>
-    <t>Parkinson's Telemonitoring</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.kaggle.com/datasets/porinitahoque/parkinsons-telemonitoring </t>
-  </si>
-  <si>
-    <t>age - Subject age
-sex - Subject gender '0' - male, '1' - female
-test_time - Time since recruitment into the trial. The integer part is the number of days since recruitment.
-motor_UPDRS - Clinician's motor UPDRS score, linearly interpolated
-total_UPDRS - Clinician's total UPDRS score, linearly interpolated
-Jitter(%),Jitter(Abs),Jitter:RAP,Jitter:PPQ5,Jitter:DDP - Several measures of variation in fundamental frequency
-Shimmer,Shimmer(dB),Shimmer:APQ3,Shimmer:APQ5,Shimmer:APQ11,Shimmer:DDA - Several measures of variation in amplitude
-NHR,HNR - Two measures of ratio of noise to tonal components in the voice
-RPDE - A nonlinear dynamical complexity measure
-DFA - Signal fractal scaling exponent
-PPE - A nonlinear measure of fundamental frequency variation</t>
+    <t>male
+age
+education
+currentSmoker
+cigsPerDay
+BPMeds
+prevalentStroke
+prevalentHyp
+diabetes
+totChol
+sysBP
+diaBP
+BMI
+heartRate
+glucose
+TenYearCHD</t>
+  </si>
+  <si>
+    <t>Pregnancies
+Glucose
+BloodPressure
+SkinThickness
+Insulin
+BMI
+DiabetesPedigreeFunction
+Age
+Outcome</t>
   </si>
 </sst>
 </file>
@@ -340,9 +344,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -364,6 +365,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -680,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD0653A2-F85B-1F4F-8AF2-A95ABD5D8D41}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -697,13 +701,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
@@ -753,19 +757,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="15" customFormat="1" ht="232" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:6" s="14" customFormat="1" ht="232" x14ac:dyDescent="0.35">
+      <c r="A5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="14" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" ht="319" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -796,20 +800,20 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="232" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
@@ -819,37 +823,23 @@
       <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" s="15" customFormat="1" ht="203" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -864,7 +854,6 @@
     <hyperlink ref="B8" r:id="rId6" xr:uid="{A463B3E8-E66D-4EF6-93D6-F8FE61F440D3}"/>
     <hyperlink ref="B9" r:id="rId7" xr:uid="{87A46C47-8126-4CF0-99CB-51A1ED1725C5}"/>
     <hyperlink ref="B10" r:id="rId8" xr:uid="{9CE3F84B-5C65-4B1D-982A-B27D7F7BEB00}"/>
-    <hyperlink ref="B11" r:id="rId9" xr:uid="{AFF6E6D3-086D-4178-8BA6-1C6D49FA4AD3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new dataset lung cancer
</commit_message>
<xml_diff>
--- a/Datasets.xlsx
+++ b/Datasets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Btech\sem8 Aroygasathi\ArogyaSathi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661CAFE4-2899-4663-8B29-B773F33FC82C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330C802A-717A-4082-ADD5-DFE48C7D70C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="14050" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Dataset study</t>
   </si>
@@ -230,6 +230,38 @@
   </si>
   <si>
     <t>Features</t>
+  </si>
+  <si>
+    <t>Lung Cancer Dataset</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/datasets/thedevastator/cancer-patients-and-air-pollution-a-new-link/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age-	The age of the patient. (Numeric)
+Gender-	The gender of the patient. (Categorical)
+Air Pollution-	The level of air pollution exposure of the patient. (Categorical)
+Alcohol use-	The level of alcohol use of the patient. (Categorical)
+Dust Allergy-	The level of dust allergy of the patient. (Categorical)
+Occupational Hazards-	The level of occupational hazards of the patient. (Categorical)
+Genetic Risk-	The level of genetic risk of the patient. (Categorical)
+chronic Lung Disease-	The level of chronic lung disease of the patient. (Categorical)
+Balanced Diet-	The level of balanced diet of the patient. (Categorical)
+Obesity-	The level of obesity of the patient. (Categorical)
+Smoking-	The level of smoking of the patient. (Categorical)
+Passive Smoker-	The level of passive smoker of the patient. (Categorical)
+Chest Pain-	The level of chest pain of the patient. (Categorical)
+Coughing of Blood-	The level of coughing of blood of the patient. (Categorical)
+Fatigue-	The level of fatigue of the patient. (Categorical)
+Weight Loss-	The level of weight loss of the patient. (Categorical)
+Shortness of Breath-	The level of shortness of breath of the patient. (Categorical)
+Wheezing-	The level of wheezing of the patient. (Categorical)
+Swallowing Difficulty-	The level of swallowing difficulty of the patient. (Categorical)
+Clubbing of Finger Nails-	The level of clubbing of finger nails of the patient. (Categorical)
+</t>
+  </si>
+  <si>
+    <t>Severiaity of Lung Cancer</t>
   </si>
 </sst>
 </file>
@@ -684,17 +716,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD0653A2-F85B-1F4F-8AF2-A95ABD5D8D41}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.1796875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="21" style="3" customWidth="1"/>
+    <col min="3" max="3" width="29.6328125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="74.7265625" style="6" customWidth="1"/>
     <col min="5" max="5" width="13.81640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="11.54296875" style="3" customWidth="1"/>
@@ -839,6 +871,20 @@
       </c>
       <c r="D10" s="5" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="319" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -854,6 +900,7 @@
     <hyperlink ref="B8" r:id="rId6" xr:uid="{A463B3E8-E66D-4EF6-93D6-F8FE61F440D3}"/>
     <hyperlink ref="B9" r:id="rId7" xr:uid="{87A46C47-8126-4CF0-99CB-51A1ED1725C5}"/>
     <hyperlink ref="B10" r:id="rId8" xr:uid="{9CE3F84B-5C65-4B1D-982A-B27D7F7BEB00}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{95DA35C2-556E-466E-AE74-1DBD56AB1DB1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>